<commit_message>
null val in filters
</commit_message>
<xml_diff>
--- a/app/parser/data.xlsx
+++ b/app/parser/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13139" uniqueCount="2925">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13138" uniqueCount="2925">
   <si>
     <t>Номер позиции</t>
   </si>
@@ -9164,7 +9164,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I1628"/>
+  <dimension ref="A1:I1627"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -53354,19 +53354,6 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="1628" customHeight="1" ht="17.25">
-      <c r="A1628" s="3"/>
-      <c r="B1628" s="3"/>
-      <c r="C1628" s="3"/>
-      <c r="D1628" s="3"/>
-      <c r="E1628" s="3"/>
-      <c r="F1628" s="3"/>
-      <c r="G1628" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1628" s="3"/>
-      <c r="I1628" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>